<commit_message>
preice with by items
</commit_message>
<xml_diff>
--- a/Girassal.Web/wwwroot/templates/fatura_p25_.xlsx
+++ b/Girassal.Web/wwwroot/templates/fatura_p25_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fausi\source\repos\Girassal.Web\Girassal.Web\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0BB8EA-3278-4442-BA56-4C472CC0BD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47497EF0-D2C0-43F8-A070-3CDB90DE5BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{3476D741-030A-4DE0-9959-743EDF208D86}"/>
+    <workbookView xWindow="3510" yWindow="-12690" windowWidth="21600" windowHeight="11295" xr2:uid="{3476D741-030A-4DE0-9959-743EDF208D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,34 +46,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Preço</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Girassol Lavandaria</t>
-  </si>
-  <si>
-    <t>AV. Ahmed Sekou /touré,</t>
-  </si>
-  <si>
-    <t>+ 258 86 085 2222</t>
   </si>
   <si>
     <t>Alto-Maé</t>
   </si>
   <si>
-    <t>Itens</t>
+    <t>nº 3479 R/C  Maputo</t>
   </si>
   <si>
-    <t>nº 3479 R/C  Maputo</t>
+    <t>cell:+258860852222</t>
+  </si>
+  <si>
+    <t>AV. Ahmed Sekou/touré,</t>
+  </si>
+  <si>
+    <t>Nuit:401376070</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,14 +93,6 @@
     <font>
       <b/>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -138,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -148,7 +137,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,38 +488,38 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:B28"/>
+  <dimension ref="A2:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -539,13 +527,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
@@ -568,14 +556,11 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>